<commit_message>
Changes in Reimb Form Object classes
</commit_message>
<xml_diff>
--- a/reimbursement/src/main/resources/TestData/CreateReimbTypes/CreateReimbTypesScenarios.xlsx
+++ b/reimbursement/src/main/resources/TestData/CreateReimbTypes/CreateReimbTypesScenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ReimbForm" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -29,9 +29,6 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Body</t>
-  </si>
-  <si>
     <t xml:space="preserve">Applicable</t>
   </si>
   <si>
@@ -44,7 +41,7 @@
     <t xml:space="preserve">Ledger</t>
   </si>
   <si>
-    <t xml:space="preserve">TestCaseName</t>
+    <t xml:space="preserve">Reimbursement_Limits</t>
   </si>
   <si>
     <t xml:space="preserve">Test_Description</t>
@@ -56,32 +53,49 @@
     <t xml:space="preserve">created through automation script</t>
   </si>
   <si>
-    <t xml:space="preserve">Create Reimb Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reimb Form auto2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group_Company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Band_grade_desig</t>
+    <t xml:space="preserve">1,2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">created Reimbursement unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Band_grade_designation</t>
   </si>
   <si>
     <t xml:space="preserve">Location</t>
   </si>
   <si>
-    <t xml:space="preserve">uppercappu</t>
+    <t xml:space="preserve">UpperCapPerUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UpperCap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoOfTimesPerMonth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxAmountPerPerson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DaysPostExpense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AutoApprovalLimit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AutoCalculate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL_0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-409]D\-MMM"/>
-    <numFmt numFmtId="166" formatCode="[$-409]M/D/YYYY"/>
+    <numFmt numFmtId="165" formatCode="[$-409]M/D/YYYY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -166,11 +180,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -191,20 +205,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -232,39 +247,22 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2"/>
       <c r="H2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -281,65 +279,68 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>